<commit_message>
Rename example to correct layers
Former-commit-id: 2db099ff672cc8bcab21f532b398dff5bed5b9f1
</commit_message>
<xml_diff>
--- a/failmap/organizations/static/example_organizations_import_file.xlsx
+++ b/failmap/organizations/static/example_organizations_import_file.xlsx
@@ -37,7 +37,7 @@
     <t>NL</t>
   </si>
   <si>
-    <t>water board</t>
+    <t>water_board</t>
   </si>
   <si>
     <t>aaenmaas.nl</t>
@@ -256,12 +256,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -274,14 +280,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -289,30 +295,15 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="9"/>
-      </right>
-      <top style="thin">
-        <color indexed="9"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -320,7 +311,22 @@
         <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -337,16 +343,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -366,6 +372,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffcacaca"/>
     </indexedColors>
@@ -566,17 +573,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -604,10 +611,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -855,12 +862,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1147,7 +1154,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1175,10 +1182,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>